<commit_message>
need improve for generic model passing to funct
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA69A59F-1D7D-4EAF-BD1E-3A21B75D0E19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC76175-20BF-4490-8260-25518F32B7E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="1305" windowWidth="8925" windowHeight="6915" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="11" r:id="rId1"/>
@@ -3063,8 +3063,8 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8168,7 +8168,7 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
next for user and profile
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC76175-20BF-4490-8260-25518F32B7E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="11" r:id="rId1"/>
@@ -56,7 +50,7 @@
     <definedName name="UNI_RET_VALUE" hidden="1">16</definedName>
     <definedName name="unit">PlantUnit!$A$2:$A$57</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -2541,9 +2535,6 @@
     <t>start1234</t>
   </si>
   <si>
-    <t>foreign_dept</t>
-  </si>
-  <si>
     <t>foreign_section</t>
   </si>
   <si>
@@ -2608,12 +2599,15 @@
   </si>
   <si>
     <t>SPV_ORG</t>
+  </si>
+  <si>
+    <t>foreign_department</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -2694,7 +2688,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2721,7 +2715,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2780,7 +2774,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2813,26 +2807,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2865,23 +2842,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3057,13 +3017,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3230,7 +3190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3251,7 +3211,7 @@
         <v>810</v>
       </c>
       <c r="B1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3806,7 +3766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4439,7 +4399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -7845,7 +7805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -7959,14 +7919,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8030,14 +7990,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8054,7 +8014,7 @@
         <v>811</v>
       </c>
       <c r="C1" t="s">
-        <v>826</v>
+        <v>848</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8162,7 +8122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1C17C0-297A-4000-BC84-C06FB38290A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8182,24 +8142,24 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>830</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>831</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>832</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>835</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>836</v>
       </c>
       <c r="D2" t="s">
         <v>819</v>
@@ -8207,13 +8167,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>836</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>835</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>837</v>
       </c>
       <c r="D3" t="s">
         <v>819</v>
@@ -8221,13 +8181,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>837</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>838</v>
       </c>
       <c r="D4" t="s">
         <v>819</v>
@@ -8235,35 +8195,35 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>838</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>837</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>839</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>838</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>840</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>839</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>841</v>
       </c>
       <c r="D7" t="s">
         <v>818</v>
@@ -8271,10 +8231,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D8" t="s">
         <v>818</v>
@@ -8286,7 +8246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8304,15 +8264,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="8" t="s">
+        <v>832</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>833</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>825</v>
@@ -8320,7 +8280,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>825</v>
@@ -8328,7 +8288,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>825</v>
@@ -8336,7 +8296,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>825</v>
@@ -8344,7 +8304,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>825</v>
@@ -8352,7 +8312,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>825</v>
@@ -8360,7 +8320,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>825</v>
@@ -8378,7 +8338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8400,37 +8360,37 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="7" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="7" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="7" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="7" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
   </sheetData>
@@ -8439,7 +8399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8546,7 +8506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8567,7 +8527,7 @@
         <v>810</v>
       </c>
       <c r="B1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -8863,7 +8823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>

</xml_diff>

<commit_message>
all configuration look ok
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1297D9-A159-4418-A46C-8DBF55A52911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="15" yWindow="1650" windowWidth="9420" windowHeight="6915" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="status" sheetId="11" r:id="rId1"/>
-    <sheet name="Department" sheetId="32" r:id="rId2"/>
-    <sheet name="Section" sheetId="33" r:id="rId3"/>
+    <sheet name="Department" sheetId="32" r:id="rId1"/>
+    <sheet name="Section" sheetId="33" r:id="rId2"/>
+    <sheet name="User" sheetId="34" r:id="rId3"/>
     <sheet name="Profile" sheetId="35" r:id="rId4"/>
-    <sheet name="User" sheetId="34" r:id="rId5"/>
-    <sheet name="group" sheetId="9" r:id="rId6"/>
-    <sheet name="PlantArea" sheetId="6" r:id="rId7"/>
-    <sheet name="PlantUnit" sheetId="8" r:id="rId8"/>
-    <sheet name="EqpCategory" sheetId="7" r:id="rId9"/>
-    <sheet name="EquipmentName" sheetId="1" r:id="rId10"/>
-    <sheet name="Sparepart" sheetId="2" r:id="rId11"/>
-    <sheet name="Tool" sheetId="3" r:id="rId12"/>
-    <sheet name="Req.Category" sheetId="10" r:id="rId13"/>
+    <sheet name="status" sheetId="11" r:id="rId5"/>
+    <sheet name="ProfileAction" sheetId="36" r:id="rId6"/>
+    <sheet name="group" sheetId="9" r:id="rId7"/>
+    <sheet name="PlantArea" sheetId="6" r:id="rId8"/>
+    <sheet name="PlantUnit" sheetId="8" r:id="rId9"/>
+    <sheet name="EqpCategory" sheetId="7" r:id="rId10"/>
+    <sheet name="EquipmentName" sheetId="1" r:id="rId11"/>
+    <sheet name="Sparepart" sheetId="2" r:id="rId12"/>
+    <sheet name="Tool" sheetId="3" r:id="rId13"/>
+    <sheet name="Req.Category" sheetId="10" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="sort">#REF!</definedName>
@@ -50,12 +57,12 @@
     <definedName name="UNI_RET_VALUE" hidden="1">16</definedName>
     <definedName name="unit">PlantUnit!$A$2:$A$57</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="854">
   <si>
     <t>Spoll reduce 6" x 3" Cat warna putih</t>
   </si>
@@ -2544,9 +2551,6 @@
     <t>foreign_category</t>
   </si>
   <si>
-    <t>foreign_user</t>
-  </si>
-  <si>
     <t>forward_path</t>
   </si>
   <si>
@@ -2602,12 +2606,30 @@
   </si>
   <si>
     <t>foreign_department</t>
+  </si>
+  <si>
+    <t>Dept. Head Production</t>
+  </si>
+  <si>
+    <t>Dept. Head Maintenance</t>
+  </si>
+  <si>
+    <t>sptdOrg</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Canceled during execution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -2657,7 +2679,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2665,12 +2687,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2685,10 +2722,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2715,7 +2755,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2774,7 +2814,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2807,9 +2847,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2842,6 +2899,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3017,19 +3091,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3042,155 +3117,124 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="B2" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>788</v>
+        <v>677</v>
       </c>
       <c r="B3" t="s">
-        <v>803</v>
+        <v>677</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="B4" t="s">
-        <v>812</v>
+        <v>780</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
       <c r="B5" t="s">
-        <v>813</v>
+        <v>783</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
       <c r="B6" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>792</v>
-      </c>
-      <c r="B7" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>793</v>
-      </c>
-      <c r="B8" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>778</v>
-      </c>
-      <c r="B9" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>794</v>
-      </c>
-      <c r="B10" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>795</v>
-      </c>
-      <c r="B11" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>773</v>
-      </c>
-      <c r="B12" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>796</v>
-      </c>
-      <c r="B13" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>797</v>
-      </c>
-      <c r="B14" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>798</v>
-      </c>
-      <c r="B15" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>799</v>
-      </c>
-      <c r="B16" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>800</v>
-      </c>
-      <c r="B17" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>801</v>
-      </c>
-      <c r="B18" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>802</v>
-      </c>
-      <c r="B19" t="s">
-        <v>802</v>
+        <v>755</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3765,8 +3809,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4398,8 +4442,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -7804,8 +7848,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -7919,85 +7963,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>810</v>
-      </c>
-      <c r="B1" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>779</v>
-      </c>
-      <c r="B2" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>677</v>
-      </c>
-      <c r="B3" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>780</v>
-      </c>
-      <c r="B4" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>783</v>
-      </c>
-      <c r="B5" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>781</v>
-      </c>
-      <c r="B6" t="s">
-        <v>781</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8014,7 +7987,7 @@
         <v>811</v>
       </c>
       <c r="C1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8114,6 +8087,28 @@
       </c>
       <c r="C10" t="s">
         <v>781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>848</v>
+      </c>
+      <c r="B11" t="s">
+        <v>848</v>
+      </c>
+      <c r="C11" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>849</v>
+      </c>
+      <c r="B12" t="s">
+        <v>849</v>
+      </c>
+      <c r="C12" t="s">
+        <v>677</v>
       </c>
     </row>
   </sheetData>
@@ -8121,15 +8116,107 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>831</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <customProperties>
+    <customPr name="WorksheetGuid" r:id="rId2"/>
+  </customProperties>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8142,98 +8229,110 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>829</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>830</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>831</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>834</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>835</v>
       </c>
       <c r="D2" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>835</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>836</v>
       </c>
       <c r="D3" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>836</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>835</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>837</v>
       </c>
       <c r="D4" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D5" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
-        <v>838</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="D6" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="10" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
-        <v>839</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>838</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>840</v>
       </c>
       <c r="D7" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7" t="s">
-        <v>840</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>839</v>
       </c>
       <c r="D8" t="s">
@@ -8246,99 +8345,378 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="8" t="s">
-        <v>832</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>833</v>
+      <c r="A1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>825</v>
+      <c r="A2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B2" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>835</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>825</v>
+      <c r="A3" t="s">
+        <v>788</v>
+      </c>
+      <c r="B3" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>825</v>
+      <c r="A4" t="s">
+        <v>789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
-        <v>837</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>825</v>
+      <c r="A5" t="s">
+        <v>790</v>
+      </c>
+      <c r="B5" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
-        <v>838</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>825</v>
+      <c r="A6" t="s">
+        <v>791</v>
+      </c>
+      <c r="B6" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="7" t="s">
-        <v>839</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>825</v>
+      <c r="A7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B7" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
-        <v>840</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>825</v>
+      <c r="A8" t="s">
+        <v>793</v>
+      </c>
+      <c r="B8" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>778</v>
+      </c>
+      <c r="B9" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B10" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>795</v>
+      </c>
+      <c r="B11" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>773</v>
+      </c>
+      <c r="B12" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>796</v>
+      </c>
+      <c r="B13" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>797</v>
+      </c>
+      <c r="B14" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>798</v>
+      </c>
+      <c r="B15" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>799</v>
+      </c>
+      <c r="B16" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>800</v>
+      </c>
+      <c r="B17" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>801</v>
+      </c>
+      <c r="B18" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>802</v>
+      </c>
+      <c r="B19" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>852</v>
+      </c>
+      <c r="B20" t="s">
+        <v>853</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <customProperties>
-    <customPr name="WorksheetGuid" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2B9D11-3559-4E5F-BE93-612A474A70D0}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B3" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B4" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B5" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B6" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B8" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B9" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B10" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B11" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B12" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B13" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B14" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B15" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="B16" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="B17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="B18" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>850</v>
+      </c>
+      <c r="B19" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="B20" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="B21" t="s">
+        <v>788</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8360,37 +8738,37 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="7" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="7" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="7" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="7" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
   </sheetData>
@@ -8398,8 +8776,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8505,8 +8883,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8820,76 +9198,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>755</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
long journey  move status, section and dept not ok
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1297D9-A159-4418-A46C-8DBF55A52911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6351BBD6-0A39-4174-A948-952D8A0B51CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="1650" windowWidth="9420" windowHeight="6915" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="32" r:id="rId1"/>
@@ -57,7 +57,17 @@
     <definedName name="UNI_RET_VALUE" hidden="1">16</definedName>
     <definedName name="unit">PlantUnit!$A$2:$A$57</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2539,9 +2549,6 @@
     <t>Part of QCAS for safety</t>
   </si>
   <si>
-    <t>start1234</t>
-  </si>
-  <si>
     <t>foreign_section</t>
   </si>
   <si>
@@ -2624,6 +2631,9 @@
   </si>
   <si>
     <t>Canceled during execution</t>
+  </si>
+  <si>
+    <t>pbkdf2_sha256$216000$bf4BjBkTHqCR$EQplucWgLJEJ+7Xg363PVHfAepOaM6n0+Kje00D2J7k=</t>
   </si>
 </sst>
 </file>
@@ -3255,7 +3265,7 @@
         <v>810</v>
       </c>
       <c r="B1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7987,7 +7997,7 @@
         <v>811</v>
       </c>
       <c r="C1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8091,10 +8101,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B11" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C11" t="s">
         <v>779</v>
@@ -8102,10 +8112,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B12" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C12" t="s">
         <v>677</v>
@@ -8124,77 +8134,77 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="109.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="8" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>831</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
-        <v>833</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>825</v>
+      <c r="B2" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>825</v>
+        <v>833</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>835</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>825</v>
+        <v>834</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>825</v>
+        <v>835</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
-        <v>837</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>825</v>
+        <v>836</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>838</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>825</v>
+        <v>837</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
-        <v>839</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>825</v>
+        <v>838</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -8229,27 +8239,27 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>828</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>829</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>830</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>833</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>833</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>834</v>
       </c>
       <c r="D2" t="s">
         <v>819</v>
@@ -8257,13 +8267,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>834</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>833</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>835</v>
       </c>
       <c r="D3" t="s">
         <v>819</v>
@@ -8271,13 +8281,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>835</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>836</v>
       </c>
       <c r="D4" t="s">
         <v>819</v>
@@ -8285,41 +8295,41 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>835</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>837</v>
-      </c>
       <c r="D5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D6" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D7" t="s">
         <v>818</v>
@@ -8327,13 +8337,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D8" t="s">
         <v>818</v>
@@ -8514,10 +8524,10 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>851</v>
+      </c>
+      <c r="B20" t="s">
         <v>852</v>
-      </c>
-      <c r="B20" t="s">
-        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -8544,15 +8554,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B2" t="s">
         <v>801</v>
@@ -8560,7 +8570,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B3" t="s">
         <v>802</v>
@@ -8568,15 +8578,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B4" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B5" t="s">
         <v>798</v>
@@ -8584,7 +8594,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="10" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B6" t="s">
         <v>799</v>
@@ -8592,7 +8602,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B7" t="s">
         <v>800</v>
@@ -8600,7 +8610,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B8" t="s">
         <v>794</v>
@@ -8608,7 +8618,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B9" t="s">
         <v>795</v>
@@ -8616,7 +8626,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B10" t="s">
         <v>773</v>
@@ -8624,7 +8634,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B11" t="s">
         <v>796</v>
@@ -8632,7 +8642,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B12" t="s">
         <v>797</v>
@@ -8640,7 +8650,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B13" t="s">
         <v>793</v>
@@ -8648,7 +8658,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B14" t="s">
         <v>793</v>
@@ -8656,7 +8666,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B15" t="s">
         <v>778</v>
@@ -8664,7 +8674,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B16" t="s">
         <v>791</v>
@@ -8672,7 +8682,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B17" t="s">
         <v>792</v>
@@ -8680,7 +8690,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B18" t="s">
         <v>789</v>
@@ -8688,7 +8698,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B19" t="s">
         <v>790</v>
@@ -8696,7 +8706,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B20" t="s">
         <v>787</v>
@@ -8704,7 +8714,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="10" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B21" t="s">
         <v>788</v>
@@ -8738,37 +8748,37 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="7" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="7" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="7" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="7" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
   </sheetData>
@@ -8905,7 +8915,7 @@
         <v>810</v>
       </c>
       <c r="B1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
good separation utility and work order
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6351BBD6-0A39-4174-A948-952D8A0B51CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB776F8-B7F6-4D94-AAAC-9E4CC6FC92E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="32" r:id="rId1"/>
     <sheet name="Section" sheetId="33" r:id="rId2"/>
     <sheet name="User" sheetId="34" r:id="rId3"/>
     <sheet name="Profile" sheetId="35" r:id="rId4"/>
-    <sheet name="status" sheetId="11" r:id="rId5"/>
-    <sheet name="ProfileAction" sheetId="36" r:id="rId6"/>
-    <sheet name="group" sheetId="9" r:id="rId7"/>
-    <sheet name="PlantArea" sheetId="6" r:id="rId8"/>
-    <sheet name="PlantUnit" sheetId="8" r:id="rId9"/>
-    <sheet name="EqpCategory" sheetId="7" r:id="rId10"/>
-    <sheet name="EquipmentName" sheetId="1" r:id="rId11"/>
-    <sheet name="Sparepart" sheetId="2" r:id="rId12"/>
-    <sheet name="Tool" sheetId="3" r:id="rId13"/>
-    <sheet name="Req.Category" sheetId="10" r:id="rId14"/>
+    <sheet name="action" sheetId="37" r:id="rId5"/>
+    <sheet name="status" sheetId="11" r:id="rId6"/>
+    <sheet name="ProfileAction" sheetId="36" r:id="rId7"/>
+    <sheet name="group" sheetId="9" r:id="rId8"/>
+    <sheet name="PlantArea" sheetId="6" r:id="rId9"/>
+    <sheet name="PlantUnit" sheetId="8" r:id="rId10"/>
+    <sheet name="EqpCategory" sheetId="7" r:id="rId11"/>
+    <sheet name="EquipmentName" sheetId="1" r:id="rId12"/>
+    <sheet name="Sparepart" sheetId="2" r:id="rId13"/>
+    <sheet name="Tool" sheetId="3" r:id="rId14"/>
+    <sheet name="Req.Category" sheetId="10" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="sort">#REF!</definedName>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="854">
   <si>
     <t>Spoll reduce 6" x 3" Cat warna putih</t>
   </si>
@@ -3172,6 +3173,323 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="42" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" customFormat="1">
+      <c r="A1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="6" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="6" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="6" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="6" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="6" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="6" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="6" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="6" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="6" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="6" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="6" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="6" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="6" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="6" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="6" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="6" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="6" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="6" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="6" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="6" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="6" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="6" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="6" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="6" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="6" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="6" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="6" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="6" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="6" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="6" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="6" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="6" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="6" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="6">
+        <f>LEN(A57)</f>
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3243,7 +3561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3819,7 +4137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -4452,7 +4770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7858,7 +8176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8133,8 +8451,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8355,6 +8673,187 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D7EE59-766E-44F5-8C91-B65E5E147CD7}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>788</v>
+      </c>
+      <c r="B3" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>790</v>
+      </c>
+      <c r="B5" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>791</v>
+      </c>
+      <c r="B6" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B7" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>793</v>
+      </c>
+      <c r="B8" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>778</v>
+      </c>
+      <c r="B9" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B10" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>795</v>
+      </c>
+      <c r="B11" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>773</v>
+      </c>
+      <c r="B12" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>796</v>
+      </c>
+      <c r="B13" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>797</v>
+      </c>
+      <c r="B14" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>798</v>
+      </c>
+      <c r="B15" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>799</v>
+      </c>
+      <c r="B16" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>800</v>
+      </c>
+      <c r="B17" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>801</v>
+      </c>
+      <c r="B18" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>802</v>
+      </c>
+      <c r="B19" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>851</v>
+      </c>
+      <c r="B20" t="s">
+        <v>852</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8535,7 +9034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2B9D11-3559-4E5F-BE93-612A474A70D0}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8725,7 +9224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8786,7 +9285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8891,321 +9390,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:B59"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="42" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" customFormat="1">
-      <c r="A1" t="s">
-        <v>810</v>
-      </c>
-      <c r="B1" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="6" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="6" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="6" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="6" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="6" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="6" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="6" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="6" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="6" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="6" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="6" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="6" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="6" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="6" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="6" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="6" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="6" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="6" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="6" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="6" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="6" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="6" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="6" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="6" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="6" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="6" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="6" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="6" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="6" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="6" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="6" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="6" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="6" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="6" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="6" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="6" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="6" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="6" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="6" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="6" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="6" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="6" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="6" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="6" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="6">
-        <f>LEN(A57)</f>
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
wo opening just working
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB776F8-B7F6-4D94-AAAC-9E4CC6FC92E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877100E4-8364-47AF-8723-098B0A3EEECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="32" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="User" sheetId="34" r:id="rId3"/>
     <sheet name="Profile" sheetId="35" r:id="rId4"/>
     <sheet name="action" sheetId="37" r:id="rId5"/>
-    <sheet name="status" sheetId="11" r:id="rId6"/>
-    <sheet name="ProfileAction" sheetId="36" r:id="rId7"/>
-    <sheet name="group" sheetId="9" r:id="rId8"/>
-    <sheet name="PlantArea" sheetId="6" r:id="rId9"/>
-    <sheet name="PlantUnit" sheetId="8" r:id="rId10"/>
-    <sheet name="EqpCategory" sheetId="7" r:id="rId11"/>
-    <sheet name="EquipmentName" sheetId="1" r:id="rId12"/>
-    <sheet name="Sparepart" sheetId="2" r:id="rId13"/>
-    <sheet name="Tool" sheetId="3" r:id="rId14"/>
-    <sheet name="Req.Category" sheetId="10" r:id="rId15"/>
+    <sheet name="mode" sheetId="38" r:id="rId6"/>
+    <sheet name="status" sheetId="11" r:id="rId7"/>
+    <sheet name="ProfileAction" sheetId="36" r:id="rId8"/>
+    <sheet name="group" sheetId="9" r:id="rId9"/>
+    <sheet name="PlantArea" sheetId="6" r:id="rId10"/>
+    <sheet name="PlantUnit" sheetId="8" r:id="rId11"/>
+    <sheet name="EqpCategory" sheetId="7" r:id="rId12"/>
+    <sheet name="EquipmentName" sheetId="1" r:id="rId13"/>
+    <sheet name="Sparepart" sheetId="2" r:id="rId14"/>
+    <sheet name="Tool" sheetId="3" r:id="rId15"/>
+    <sheet name="Req.Category" sheetId="10" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="sort">#REF!</definedName>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="858">
   <si>
     <t>Spoll reduce 6" x 3" Cat warna putih</t>
   </si>
@@ -2635,6 +2636,18 @@
   </si>
   <si>
     <t>pbkdf2_sha256$216000$bf4BjBkTHqCR$EQplucWgLJEJ+7Xg363PVHfAepOaM6n0+Kje00D2J7k=</t>
+  </si>
+  <si>
+    <t>foreign_mode</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Stay</t>
   </si>
 </sst>
 </file>
@@ -3173,6 +3186,113 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>680</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3489,7 +3609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3561,7 +3681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -4137,7 +4257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -4770,7 +4890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8176,7 +8296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8544,7 +8664,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8677,10 +8797,251 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="C1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>788</v>
+      </c>
+      <c r="B3" t="s">
+        <v>855</v>
+      </c>
+      <c r="C3" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>856</v>
+      </c>
+      <c r="C4" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>790</v>
+      </c>
+      <c r="B5" t="s">
+        <v>855</v>
+      </c>
+      <c r="C5" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>791</v>
+      </c>
+      <c r="B6" t="s">
+        <v>856</v>
+      </c>
+      <c r="C6" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B7" t="s">
+        <v>855</v>
+      </c>
+      <c r="C7" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>793</v>
+      </c>
+      <c r="B8" t="s">
+        <v>856</v>
+      </c>
+      <c r="C8" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>778</v>
+      </c>
+      <c r="B9" t="s">
+        <v>855</v>
+      </c>
+      <c r="C9" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B10" t="s">
+        <v>857</v>
+      </c>
+      <c r="C10" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>795</v>
+      </c>
+      <c r="B11" t="s">
+        <v>857</v>
+      </c>
+      <c r="C11" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>773</v>
+      </c>
+      <c r="B12" t="s">
+        <v>857</v>
+      </c>
+      <c r="C12" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>796</v>
+      </c>
+      <c r="B13" t="s">
+        <v>857</v>
+      </c>
+      <c r="C13" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>797</v>
+      </c>
+      <c r="B14" t="s">
+        <v>855</v>
+      </c>
+      <c r="C14" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>798</v>
+      </c>
+      <c r="B15" t="s">
+        <v>856</v>
+      </c>
+      <c r="C15" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>799</v>
+      </c>
+      <c r="B16" t="s">
+        <v>856</v>
+      </c>
+      <c r="C16" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>800</v>
+      </c>
+      <c r="B17" t="s">
+        <v>855</v>
+      </c>
+      <c r="C17" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>801</v>
+      </c>
+      <c r="B18" t="s">
+        <v>856</v>
+      </c>
+      <c r="C18" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>802</v>
+      </c>
+      <c r="B19" t="s">
+        <v>857</v>
+      </c>
+      <c r="C19" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>851</v>
+      </c>
+      <c r="B20" t="s">
+        <v>856</v>
+      </c>
+      <c r="C20" t="s">
+        <v>852</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00B35F5-79EC-470D-B5D8-96EDE061CF0E}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8688,164 +9049,24 @@
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>810</v>
       </c>
-      <c r="B1" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>787</v>
-      </c>
-      <c r="B2" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>788</v>
-      </c>
-      <c r="B3" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>789</v>
-      </c>
-      <c r="B4" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>790</v>
-      </c>
-      <c r="B5" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>791</v>
-      </c>
-      <c r="B6" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>792</v>
-      </c>
-      <c r="B7" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>793</v>
-      </c>
-      <c r="B8" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>778</v>
-      </c>
-      <c r="B9" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>794</v>
-      </c>
-      <c r="B10" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>795</v>
-      </c>
-      <c r="B11" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>773</v>
-      </c>
-      <c r="B12" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>796</v>
-      </c>
-      <c r="B13" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>797</v>
-      </c>
-      <c r="B14" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>798</v>
-      </c>
-      <c r="B15" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>799</v>
-      </c>
-      <c r="B16" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>800</v>
-      </c>
-      <c r="B17" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>801</v>
-      </c>
-      <c r="B18" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>802</v>
-      </c>
-      <c r="B19" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>851</v>
-      </c>
-      <c r="B20" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -8853,7 +9074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9034,7 +9255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2B9D11-3559-4E5F-BE93-612A474A70D0}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9224,7 +9445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9283,111 +9504,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:A17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>680</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
wo summary report include wo category look ok
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -1,37 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms\mediafiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AADB262-51E1-4C0E-BC6F-481374B3AD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="495" windowWidth="9600" windowHeight="11670" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="495" windowWidth="9600" windowHeight="11670"/>
   </bookViews>
   <sheets>
-    <sheet name="Department" sheetId="32" r:id="rId1"/>
-    <sheet name="Section" sheetId="33" r:id="rId2"/>
-    <sheet name="User" sheetId="34" r:id="rId3"/>
-    <sheet name="Profile" sheetId="35" r:id="rId4"/>
-    <sheet name="Wo_priority" sheetId="39" r:id="rId5"/>
-    <sheet name="mode" sheetId="38" r:id="rId6"/>
-    <sheet name="action" sheetId="37" r:id="rId7"/>
-    <sheet name="CategoryAction" sheetId="40" r:id="rId8"/>
-    <sheet name="ProfileAction" sheetId="36" r:id="rId9"/>
-    <sheet name="group" sheetId="9" r:id="rId10"/>
-    <sheet name="PlantArea" sheetId="6" r:id="rId11"/>
-    <sheet name="PlantUnit" sheetId="8" r:id="rId12"/>
-    <sheet name="EqpCategory" sheetId="7" r:id="rId13"/>
-    <sheet name="EquipmentName" sheetId="1" r:id="rId14"/>
-    <sheet name="Sparepart" sheetId="2" r:id="rId15"/>
-    <sheet name="Tool" sheetId="3" r:id="rId16"/>
-    <sheet name="Req.Category" sheetId="10" r:id="rId17"/>
+    <sheet name="DbSetup" sheetId="42" r:id="rId1"/>
+    <sheet name="Department" sheetId="32" r:id="rId2"/>
+    <sheet name="Section" sheetId="33" r:id="rId3"/>
+    <sheet name="User" sheetId="34" r:id="rId4"/>
+    <sheet name="Profile" sheetId="35" r:id="rId5"/>
+    <sheet name="Wo_priority" sheetId="39" r:id="rId6"/>
+    <sheet name="mode" sheetId="38" r:id="rId7"/>
+    <sheet name="action" sheetId="37" r:id="rId8"/>
+    <sheet name="Category" sheetId="41" r:id="rId9"/>
+    <sheet name="CategoryAction" sheetId="40" r:id="rId10"/>
+    <sheet name="ProfileAction" sheetId="36" r:id="rId11"/>
+    <sheet name="group" sheetId="9" r:id="rId12"/>
+    <sheet name="PlantArea" sheetId="6" r:id="rId13"/>
+    <sheet name="PlantUnit" sheetId="8" r:id="rId14"/>
+    <sheet name="EqpCategory" sheetId="7" r:id="rId15"/>
+    <sheet name="EquipmentName" sheetId="1" r:id="rId16"/>
+    <sheet name="Sparepart" sheetId="2" r:id="rId17"/>
+    <sheet name="Tool" sheetId="3" r:id="rId18"/>
+    <sheet name="Req.Category" sheetId="10" r:id="rId19"/>
   </sheets>
   <definedNames>
+    <definedName name="sort" localSheetId="8">#REF!</definedName>
     <definedName name="sort">#REF!</definedName>
     <definedName name="UNI_FILT_OFFSPEC" hidden="1">2</definedName>
     <definedName name="UNI_FILT_ONSPEC" hidden="1">1</definedName>
@@ -60,7 +57,7 @@
     <definedName name="UNI_RET_VALUE" hidden="1">16</definedName>
     <definedName name="unit">PlantUnit!$A$2:$A$57</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -75,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="879">
   <si>
     <t>Spoll reduce 6" x 3" Cat warna putih</t>
   </si>
@@ -2685,12 +2682,39 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>CategoryAction</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>ProfileAction</t>
+  </si>
+  <si>
+    <t>Wo_priority</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="10"/>
@@ -2797,7 +2821,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2824,7 +2848,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2883,7 +2907,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2916,26 +2940,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2968,23 +2975,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3160,86 +3150,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="15">
+    <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
         <v>810</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>862</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>779</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>863</v>
-      </c>
-      <c r="C2" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>677</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>864</v>
-      </c>
-      <c r="C3" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>780</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>865</v>
-      </c>
-      <c r="C4" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>783</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>866</v>
-      </c>
-      <c r="C5" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>781</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>867</v>
-      </c>
-      <c r="C6" t="s">
-        <v>781</v>
+    </row>
+    <row r="2" spans="1:1" ht="15">
+      <c r="A2" s="11" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15">
+      <c r="A3" s="11" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15">
+      <c r="A4" s="11" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15">
+      <c r="A5" s="11" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15">
+      <c r="A6" s="11" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15">
+      <c r="A7" s="11" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15">
+      <c r="A8" s="11" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15">
+      <c r="A9" s="11" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15">
+      <c r="A10" s="11" t="s">
+        <v>878</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15">
+      <c r="A2" s="11" t="s">
+        <v>869</v>
+      </c>
+      <c r="B2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15">
+      <c r="A3" s="11" t="s">
+        <v>869</v>
+      </c>
+      <c r="B3" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15">
+      <c r="A4" s="11" t="s">
+        <v>869</v>
+      </c>
+      <c r="B4" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
+      <c r="A5" s="11" t="s">
+        <v>869</v>
+      </c>
+      <c r="B5" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="A6" s="11" t="s">
+        <v>801</v>
+      </c>
+      <c r="B6" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="A7" s="11" t="s">
+        <v>801</v>
+      </c>
+      <c r="B7" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="B8" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="B9" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="B10" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="11" t="s">
+        <v>787</v>
+      </c>
+      <c r="B11" t="s">
+        <v>787</v>
       </c>
     </row>
   </sheetData>
@@ -3248,8 +3327,198 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="B2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="B3" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="B4" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B5" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B6" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B8" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B9" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B10" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B11" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B12" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B13" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B14" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B15" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B16" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="B18" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="B19" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="B20" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="B21" t="s">
+        <v>788</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3309,8 +3578,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3416,8 +3685,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3733,8 +4002,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -3805,8 +4074,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4381,8 +4650,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -5014,8 +5283,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8420,8 +8689,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8535,7 +8804,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="15">
+      <c r="A1" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>779</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="C2" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="C3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>780</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="C4" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>783</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="C5" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>781</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="C6" t="s">
+        <v>781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8688,8 +9046,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8780,8 +9138,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8916,8 +9274,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78484E6D-56D5-4036-971F-D5243759599D}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -8993,8 +9351,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00B35F5-79EC-470D-B5D8-96EDE061CF0E}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -9034,8 +9392,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D7EE59-766E-44F5-8C91-B65E5E147CD7}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -9275,15 +9633,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0742416-0067-4A3B-9236-19452A9BE01A}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9291,91 +9649,28 @@
     <col min="1" max="1" width="17.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
         <v>810</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15">
+    </row>
+    <row r="2" spans="1:1" ht="15">
       <c r="A2" s="11" t="s">
         <v>869</v>
       </c>
-      <c r="B2" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15">
+    </row>
+    <row r="3" spans="1:1" ht="15">
       <c r="A3" s="11" t="s">
-        <v>869</v>
-      </c>
-      <c r="B3" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15">
       <c r="A4" s="11" t="s">
-        <v>869</v>
-      </c>
-      <c r="B4" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15">
       <c r="A5" s="11" t="s">
-        <v>869</v>
-      </c>
-      <c r="B5" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15">
-      <c r="A6" s="11" t="s">
-        <v>801</v>
-      </c>
-      <c r="B6" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15">
-      <c r="A7" s="11" t="s">
-        <v>801</v>
-      </c>
-      <c r="B7" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15">
-      <c r="A8" s="11" t="s">
-        <v>797</v>
-      </c>
-      <c r="B8" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15">
-      <c r="A9" s="11" t="s">
-        <v>797</v>
-      </c>
-      <c r="B9" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15">
-      <c r="A10" s="11" t="s">
-        <v>797</v>
-      </c>
-      <c r="B10" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15">
-      <c r="A11" s="11" t="s">
-        <v>787</v>
-      </c>
-      <c r="B11" t="s">
         <v>787</v>
       </c>
     </row>
@@ -9383,194 +9678,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2B9D11-3559-4E5F-BE93-612A474A70D0}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1">
-      <c r="A1" s="7" t="s">
-        <v>830</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="B2" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="B3" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="B4" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
-        <v>833</v>
-      </c>
-      <c r="B5" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="10" t="s">
-        <v>833</v>
-      </c>
-      <c r="B6" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="10" t="s">
-        <v>833</v>
-      </c>
-      <c r="B7" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="B8" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="B9" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="B10" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="B11" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="B12" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="B13" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="10" t="s">
-        <v>835</v>
-      </c>
-      <c r="B14" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="10" t="s">
-        <v>835</v>
-      </c>
-      <c r="B15" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="B16" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="B17" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="10" t="s">
-        <v>849</v>
-      </c>
-      <c r="B18" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="10" t="s">
-        <v>849</v>
-      </c>
-      <c r="B19" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="10" t="s">
-        <v>838</v>
-      </c>
-      <c r="B20" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="10" t="s">
-        <v>838</v>
-      </c>
-      <c r="B21" t="s">
-        <v>788</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>